<commit_message>
added labels to painting list
</commit_message>
<xml_diff>
--- a/paintingList.xlsx
+++ b/paintingList.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="18540" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="158">
   <si>
     <t>Title</t>
   </si>
@@ -25,6 +30,12 @@
     <t>Gallery</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
     <t>After Many Days</t>
   </si>
   <si>
@@ -470,13 +481,25 @@
   </si>
   <si>
     <t>Giuliano Burgiardini</t>
+  </si>
+  <si>
+    <t>hA+</t>
+  </si>
+  <si>
+    <t>hA-</t>
+  </si>
+  <si>
+    <t>lA+</t>
+  </si>
+  <si>
+    <t>lA-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -826,14 +849,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -843,1128 +866,1619 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>3003</v>
+      </c>
+      <c r="F2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>1009</v>
+      </c>
+      <c r="F3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>3002</v>
+      </c>
+      <c r="F4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D5">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>10004</v>
+      </c>
+      <c r="F5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D6">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>1621</v>
+      </c>
+      <c r="F6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>1001</v>
+      </c>
+      <c r="F7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D8">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>1613</v>
+      </c>
+      <c r="F8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>3001</v>
+      </c>
+      <c r="F9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>95</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D10">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>10003</v>
+      </c>
+      <c r="F10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>2008</v>
+      </c>
+      <c r="F11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>103</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D12">
         <v>200</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>20001</v>
+      </c>
+      <c r="F12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>2015</v>
+      </c>
+      <c r="F13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>1007</v>
+      </c>
+      <c r="F14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D15">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>10005</v>
+      </c>
+      <c r="F15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D16">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>10001</v>
+      </c>
+      <c r="F16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>1010</v>
+      </c>
+      <c r="F17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>2010</v>
+      </c>
+      <c r="F18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D19">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>1906</v>
+      </c>
+      <c r="F19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>108</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D20">
         <v>200</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>20006</v>
+      </c>
+      <c r="F20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21">
+        <v>2016</v>
+      </c>
+      <c r="F21" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D22">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>1606</v>
+      </c>
+      <c r="F22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D23">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <v>1628</v>
+      </c>
+      <c r="F23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D24">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <v>1604</v>
+      </c>
+      <c r="F24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>1023</v>
+      </c>
+      <c r="F25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D26">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>1609</v>
+      </c>
+      <c r="F26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D27">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>1618</v>
+      </c>
+      <c r="F27" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>91</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <v>3009</v>
+      </c>
+      <c r="F28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29">
+        <v>2012</v>
+      </c>
+      <c r="F29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30">
+        <v>1013</v>
+      </c>
+      <c r="F30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D31">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31">
+        <v>1603</v>
+      </c>
+      <c r="F31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D32">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32">
+        <v>1909</v>
+      </c>
+      <c r="F32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>87</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33">
+        <v>3005</v>
+      </c>
+      <c r="F33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34">
+        <v>2013</v>
+      </c>
+      <c r="F34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35">
+        <v>1017</v>
+      </c>
+      <c r="F35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="1">
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36">
+        <v>1005</v>
+      </c>
+      <c r="F36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="1">
         <v>107</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D37">
         <v>200</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37">
+        <v>20005</v>
+      </c>
+      <c r="F37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="1">
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D38">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38">
+        <v>1612</v>
+      </c>
+      <c r="F38" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="1">
         <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39">
+        <v>2006</v>
+      </c>
+      <c r="F39" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="1">
         <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40">
+        <v>1016</v>
+      </c>
+      <c r="F40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="1">
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41">
+        <v>1002</v>
+      </c>
+      <c r="F41" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="1">
         <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D42">
         <v>16</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42">
+        <v>1626</v>
+      </c>
+      <c r="F42" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="1">
         <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D43">
         <v>19</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43">
+        <v>1912</v>
+      </c>
+      <c r="F43" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="1">
         <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D44">
         <v>16</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44">
+        <v>1615</v>
+      </c>
+      <c r="F44" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="1">
         <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45">
+        <v>1022</v>
+      </c>
+      <c r="F45" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="1">
         <v>100</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D46">
         <v>100</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46">
+        <v>10008</v>
+      </c>
+      <c r="F46" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="1">
         <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47">
+        <v>1011</v>
+      </c>
+      <c r="F47" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="1">
         <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D48">
         <v>16</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48">
+        <v>1622</v>
+      </c>
+      <c r="F48" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D49">
         <v>16</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49">
+        <v>1624</v>
+      </c>
+      <c r="F49" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="1">
         <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D50">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50">
+        <v>3007</v>
+      </c>
+      <c r="F50" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="1">
         <v>18</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51">
+        <v>1019</v>
+      </c>
+      <c r="F51" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="1">
         <v>102</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D52">
         <v>100</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52">
+        <v>10010</v>
+      </c>
+      <c r="F52" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="1">
         <v>101</v>
       </c>
       <c r="B53" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D53">
         <v>100</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53">
+        <v>10009</v>
+      </c>
+      <c r="F53" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="1">
         <v>82</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C54" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D54">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54">
+        <v>2019</v>
+      </c>
+      <c r="F54" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="1">
         <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C55" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D55">
         <v>19</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55">
+        <v>1908</v>
+      </c>
+      <c r="F55" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="1">
         <v>105</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D56">
         <v>200</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56">
+        <v>20003</v>
+      </c>
+      <c r="F56" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="1">
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C57" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57">
+        <v>1012</v>
+      </c>
+      <c r="F57" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="1">
         <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C58" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D58">
         <v>19</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58">
+        <v>1910</v>
+      </c>
+      <c r="F58" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="1">
         <v>99</v>
       </c>
       <c r="B59" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D59">
         <v>100</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59">
+        <v>10007</v>
+      </c>
+      <c r="F59" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="1">
         <v>104</v>
       </c>
       <c r="B60" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C60" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D60">
         <v>200</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60">
+        <v>20002</v>
+      </c>
+      <c r="F60" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="1">
         <v>94</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D61">
         <v>100</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61">
+        <v>10002</v>
+      </c>
+      <c r="F61" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="1">
         <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C62" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D62">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="E62">
+        <v>2002</v>
+      </c>
+      <c r="F62" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" s="1">
         <v>13</v>
       </c>
       <c r="B63" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C63" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="E63">
+        <v>1014</v>
+      </c>
+      <c r="F63" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="1">
         <v>33</v>
       </c>
       <c r="B64" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C64" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D64">
         <v>16</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="E64">
+        <v>1610</v>
+      </c>
+      <c r="F64" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="1">
         <v>5</v>
       </c>
       <c r="B65" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C65" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65">
+        <v>1006</v>
+      </c>
+      <c r="F65" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" s="1">
         <v>24</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C66" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D66">
         <v>16</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="E66">
+        <v>1601</v>
+      </c>
+      <c r="F66" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" s="1">
         <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C67" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67">
+        <v>2007</v>
+      </c>
+      <c r="F67" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" s="1">
         <v>42</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D68">
         <v>16</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="E68">
+        <v>1619</v>
+      </c>
+      <c r="F68" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" s="1">
         <v>54</v>
       </c>
       <c r="B69" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C69" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D69">
         <v>19</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="E69">
+        <v>1903</v>
+      </c>
+      <c r="F69" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" s="1">
         <v>74</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C70" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D70">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="E70">
+        <v>2011</v>
+      </c>
+      <c r="F70" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" s="1">
         <v>66</v>
       </c>
       <c r="B71" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D71">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="E71">
+        <v>2003</v>
+      </c>
+      <c r="F71" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" s="1">
         <v>50</v>
       </c>
       <c r="B72" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C72" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D72">
         <v>16</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="E72">
+        <v>1627</v>
+      </c>
+      <c r="F72" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" s="1">
         <v>39</v>
       </c>
       <c r="B73" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C73" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D73">
         <v>16</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="E73">
+        <v>1616</v>
+      </c>
+      <c r="F73" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" s="1">
         <v>40</v>
       </c>
       <c r="B74" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C74" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D74">
         <v>16</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="E74">
+        <v>1617</v>
+      </c>
+      <c r="F74" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" s="1">
         <v>48</v>
       </c>
       <c r="B75" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C75" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D75">
         <v>16</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="E75">
+        <v>1625</v>
+      </c>
+      <c r="F75" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" s="1">
         <v>80</v>
       </c>
       <c r="B76" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C76" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D76">
         <v>2</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="E76">
+        <v>2017</v>
+      </c>
+      <c r="F76" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77" s="1">
         <v>31</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C77" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D77">
         <v>16</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="E77">
+        <v>1608</v>
+      </c>
+      <c r="F77" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78" s="1">
         <v>28</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C78" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D78">
         <v>16</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="E78">
+        <v>1605</v>
+      </c>
+      <c r="F78" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" s="1">
         <v>43</v>
       </c>
       <c r="B79" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C79" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D79">
         <v>16</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="E79">
+        <v>1620</v>
+      </c>
+      <c r="F79" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80" s="1">
         <v>30</v>
       </c>
       <c r="B80" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C80" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D80">
         <v>16</v>
       </c>
-    </row>
-    <row r="81" spans="1:4">
+      <c r="E80">
+        <v>1607</v>
+      </c>
+      <c r="F80" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" s="1">
         <v>23</v>
       </c>
       <c r="B81" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C81" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D81">
         <v>1</v>
       </c>
+      <c r="E81">
+        <v>1024</v>
+      </c>
+      <c r="F81" t="s">
+        <v>157</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>